<commit_message>
Build(payment):Add payment to finance part
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="宏途清运终点对账单" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="宏途清运起点对账单" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -71,11 +71,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,13 @@
     <col width="8.49" customWidth="1" min="9" max="9"/>
     <col width="16.87" customWidth="1" min="10" max="10"/>
     <col width="10.58" customWidth="1" min="11" max="11"/>
+    <col width="16.87" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>宏途清运终点对账单</t>
+          <t>宏途清运起点对账单</t>
         </is>
       </c>
     </row>
@@ -485,26 +486,19 @@
       </c>
       <c r="B2" s="2" t="n"/>
       <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>阳光体育</t>
-        </is>
-      </c>
+      <c r="D2" s="2" t="n"/>
       <c r="E2" s="2" t="n"/>
       <c r="F2" s="2" t="inlineStr">
         <is>
           <t>项 目 老 板 名 称</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>刘老板</t>
-        </is>
-      </c>
+      <c r="G2" s="2" t="n"/>
       <c r="H2" s="2" t="n"/>
       <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
       <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
     </row>
     <row r="3" ht="25" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -526,6 +520,7 @@
       <c r="I3" s="2" t="n"/>
       <c r="J3" s="2" t="n"/>
       <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -555,6 +550,7 @@
       <c r="I4" s="2" t="n"/>
       <c r="J4" s="2" t="n"/>
       <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3" t="inlineStr">
@@ -600,7 +596,7 @@
       </c>
       <c r="J5" s="3" t="inlineStr">
         <is>
-          <t>终点付费金额</t>
+          <t>工地承接单价</t>
         </is>
       </c>
       <c r="K5" s="3" t="inlineStr">
@@ -608,9 +604,11 @@
           <t>总金额</t>
         </is>
       </c>
-      <c r="L5" s="3" t="n"/>
-      <c r="M5" s="3" t="n"/>
-      <c r="N5" s="3" t="n"/>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>起点补贴金额</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="4" t="n">
@@ -618,13 +616,13 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-07-31</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>彭墩</t>
+          <t>云谷人行道</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -632,7 +630,11 @@
           <t>垃圾</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr"/>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>闽HSH072</t>
+        </is>
+      </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
           <t>自带机械</t>
@@ -643,413 +645,233 @@
       </c>
       <c r="I6" s="4" t="inlineStr">
         <is>
-          <t>工地</t>
+          <t>车</t>
         </is>
       </c>
       <c r="J6" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="L6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="4" t="n">
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>总 计 金 额</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>总 计 大 写 (金 额)</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>贰佰陆拾</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="n"/>
+      <c r="I7" s="4" t="n"/>
+      <c r="J7" s="4" t="n"/>
+      <c r="K7" s="4" t="n"/>
+      <c r="L7" s="4" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>运输品类合计</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>序号</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>运输起点</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>品类</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>车队</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>总金额</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>起点补贴金额</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="C9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>云谷人行道</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>垃圾</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>闽HSH072</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="H9" s="4" t="n"/>
+      <c r="I9" s="4" t="n"/>
+      <c r="J9" s="4" t="n"/>
+      <c r="K9" s="4" t="n"/>
+      <c r="L9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="4" t="n"/>
-      <c r="M6" s="4" t="n"/>
-      <c r="N6" s="4" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>彭墩</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>垃圾</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr"/>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>自带机械</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>吨</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L7" s="4" t="n"/>
-      <c r="M7" s="4" t="n"/>
-      <c r="N7" s="4" t="n"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>2024-08-04</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>彭墩</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>垃圾</t>
-        </is>
-      </c>
-      <c r="F8" s="4" t="inlineStr">
-        <is>
-          <t>闽HRSR896</t>
-        </is>
-      </c>
-      <c r="G8" s="4" t="inlineStr">
-        <is>
-          <t>自带机械</t>
-        </is>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4" t="inlineStr">
-        <is>
-          <t>吨</t>
-        </is>
-      </c>
-      <c r="J8" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="K8" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="L8" s="4" t="n"/>
-      <c r="M8" s="4" t="n"/>
-      <c r="N8" s="4" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>2024-08-06</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="4" t="inlineStr">
-        <is>
-          <t>彭墩</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t>砖</t>
-        </is>
-      </c>
-      <c r="F9" s="4" t="inlineStr">
-        <is>
-          <t>闽HYZ633，闽HRT560，闽HRSR896，闽HPUY732</t>
-        </is>
-      </c>
-      <c r="G9" s="4" t="inlineStr">
-        <is>
-          <t>工地机械</t>
-        </is>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="I9" s="4" t="inlineStr">
-        <is>
-          <t>吨</t>
-        </is>
-      </c>
-      <c r="J9" s="4" t="n">
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" s="6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>260</v>
+      </c>
+      <c r="H10" s="6" t="n"/>
+      <c r="I10" s="6" t="n"/>
+      <c r="J10" s="6" t="n"/>
+      <c r="K10" s="6" t="n"/>
+      <c r="L10" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4" t="n"/>
-      <c r="M9" s="4" t="n"/>
-      <c r="N9" s="4" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>总 计 金 额</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n">
-        <v>110</v>
-      </c>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="inlineStr">
-        <is>
-          <t>总 计 大 写 (金 额)</t>
-        </is>
-      </c>
-      <c r="G10" s="5" t="inlineStr">
-        <is>
-          <t>壹佰壹拾</t>
-        </is>
-      </c>
-      <c r="H10" s="5" t="n"/>
-      <c r="I10" s="5" t="n"/>
-      <c r="J10" s="5" t="n"/>
-      <c r="K10" s="5" t="n"/>
-      <c r="L10" s="5" t="n"/>
-      <c r="M10" s="5" t="n"/>
-      <c r="N10" s="5" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>运输品类合计</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>序号</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>运输起点</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>品类</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>车队</t>
-        </is>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>总金额</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n"/>
-      <c r="I11" s="2" t="n"/>
-      <c r="J11" s="2" t="n"/>
-      <c r="K11" s="2" t="n"/>
-      <c r="L11" s="2" t="n"/>
-      <c r="M11" s="2" t="n"/>
-      <c r="N11" s="2" t="n"/>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>工 地 负 责 人（ 签 字 确 认 ) ：</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n"/>
+      <c r="C11" s="7" t="n"/>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="7" t="n"/>
+      <c r="F11" s="7" t="inlineStr">
+        <is>
+          <t>运 输 单 位 负 责 人 (  签 字 确 认 ) ：</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="n"/>
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
+      <c r="K11" s="7" t="n"/>
+      <c r="L11" s="7" t="n"/>
     </row>
     <row r="12" ht="15" customHeight="1">
-      <c r="C12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="inlineStr">
-        <is>
-          <t>彭墩</t>
-        </is>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>垃圾</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="inlineStr">
-        <is>
-          <t>闽HRSR896</t>
-        </is>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>110</v>
-      </c>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="4" t="n"/>
-      <c r="J12" s="4" t="n"/>
-      <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
-      <c r="N12" s="4" t="n"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="C13" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="4" t="inlineStr">
-        <is>
-          <t>彭墩</t>
-        </is>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>砖</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="inlineStr">
-        <is>
-          <t>闽HRT560，闽HRSR896，闽HPUY732</t>
-        </is>
-      </c>
-      <c r="G13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="n"/>
-      <c r="I13" s="4" t="n"/>
-      <c r="J13" s="4" t="n"/>
-      <c r="K13" s="4" t="n"/>
-      <c r="L13" s="4" t="n"/>
-      <c r="M13" s="4" t="n"/>
-      <c r="N13" s="4" t="n"/>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>合计</t>
-        </is>
-      </c>
-      <c r="D14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>110</v>
-      </c>
-      <c r="H14" s="5" t="n"/>
-      <c r="I14" s="5" t="n"/>
-      <c r="J14" s="5" t="n"/>
-      <c r="K14" s="5" t="n"/>
-      <c r="L14" s="5" t="n"/>
-      <c r="M14" s="5" t="n"/>
-      <c r="N14" s="5" t="n"/>
-    </row>
-    <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="7" t="inlineStr">
-        <is>
-          <t>工 地 负 责 人（ 签 字 确 认 ) ：</t>
-        </is>
-      </c>
-      <c r="B15" s="7" t="n"/>
-      <c r="C15" s="7" t="n"/>
-      <c r="D15" s="7" t="n"/>
-      <c r="E15" s="7" t="n"/>
-      <c r="F15" s="7" t="inlineStr">
-        <is>
-          <t>运 输 单 位 负 责 人 (  签 字 确 认 ) ：</t>
-        </is>
-      </c>
-      <c r="G15" s="7" t="n"/>
-      <c r="H15" s="7" t="n"/>
-      <c r="I15" s="7" t="n"/>
-      <c r="J15" s="7" t="n"/>
-      <c r="K15" s="7" t="n"/>
-      <c r="L15" s="7" t="n"/>
-      <c r="M15" s="7" t="n"/>
-      <c r="N15" s="7" t="n"/>
-    </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="8" t="inlineStr">
+      <c r="A12" s="8" t="inlineStr">
         <is>
           <t>经 营 范 围 ： 建筑垃圾清运，砂石料运输及销售，供应铺路石渣，云梯车租赁。</t>
         </is>
       </c>
-      <c r="B16" s="8" t="n"/>
-      <c r="C16" s="8" t="n"/>
-      <c r="D16" s="8" t="n"/>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
-      <c r="G16" s="8" t="n"/>
-      <c r="H16" s="8" t="n"/>
-      <c r="I16" s="8" t="n"/>
-      <c r="J16" s="8" t="n"/>
-      <c r="K16" s="8" t="n"/>
-      <c r="L16" s="8" t="n"/>
-      <c r="M16" s="8" t="n"/>
-      <c r="N16" s="8" t="n"/>
-    </row>
-    <row r="17" ht="22" customHeight="1">
-      <c r="A17" s="9" t="inlineStr">
+      <c r="B12" s="8" t="n"/>
+      <c r="C12" s="8" t="n"/>
+      <c r="D12" s="8" t="n"/>
+      <c r="E12" s="8" t="n"/>
+      <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
+      <c r="H12" s="8" t="n"/>
+      <c r="I12" s="8" t="n"/>
+      <c r="J12" s="8" t="n"/>
+      <c r="K12" s="8" t="n"/>
+      <c r="L12" s="8" t="n"/>
+    </row>
+    <row r="13" ht="22" customHeight="1">
+      <c r="A13" s="9" t="inlineStr">
         <is>
           <t>立 信 于 心 ， 尽 责 至 善！</t>
         </is>
       </c>
-      <c r="B17" s="9" t="n"/>
-      <c r="C17" s="9" t="n"/>
-      <c r="D17" s="9" t="n"/>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-      <c r="G17" s="9" t="n"/>
-      <c r="H17" s="9" t="n"/>
-      <c r="I17" s="9" t="n"/>
-      <c r="J17" s="9" t="n"/>
-      <c r="K17" s="9" t="n"/>
-      <c r="L17" s="9" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
+      <c r="B13" s="9" t="n"/>
+      <c r="C13" s="9" t="n"/>
+      <c r="D13" s="9" t="n"/>
+      <c r="E13" s="9" t="n"/>
+      <c r="F13" s="9" t="n"/>
+      <c r="G13" s="9" t="n"/>
+      <c r="H13" s="9" t="n"/>
+      <c r="I13" s="9" t="n"/>
+      <c r="J13" s="9" t="n"/>
+      <c r="K13" s="9" t="n"/>
+      <c r="L13" s="9" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G11:K11"/>
+  <mergeCells count="23">
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G8:K8"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A12:L12"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="G4:L4"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A13:L13"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="A8:B10"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A11:B14"/>
+    <mergeCell ref="G2:L2"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G7:L7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>